<commit_message>
data_analysis_requires_update.xlsx | updated y axis for box plot in second sheet
</commit_message>
<xml_diff>
--- a/Ibrahim_210029073_findings/data_analysis_requires_update.xlsx
+++ b/Ibrahim_210029073_findings/data_analysis_requires_update.xlsx
@@ -593,7 +593,746 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" lang="en-GB" sz="1800" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" lang="en-GB" sz="1800" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>User Performance - Age 18-30</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="50"/>
+            <c:spPr>
+              <a:ln w="9360">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Browse Products</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add Item to Basket</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>View Recommended Products</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Visit Dietary Features</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Set Preferences from Settings</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$38:$F$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="c0504d"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Browse Products</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add Item to Basket</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>View Recommended Products</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Visit Dietary Features</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Set Preferences from Settings</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$39:$F$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Median</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="9bbb59"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Browse Products</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add Item to Basket</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>View Recommended Products</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Visit Dietary Features</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Set Preferences from Settings</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$40:$F$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Q3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="8064a2"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="plus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="0"/>
+            <c:val val="100"/>
+            <c:spPr>
+              <a:ln w="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Browse Products</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add Item to Basket</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>View Recommended Products</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Visit Dietary Features</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Set Preferences from Settings</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$41:$F$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Browse Products</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Add Item to Basket</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>View Recommended Products</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Visit Dietary Features</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Set Preferences from Settings</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$42:$F$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="64815428"/>
+        <c:axId val="65542664"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="64815428"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Test Type</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65542664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65542664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="878787"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="1" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Number of Successfully passed candodates per test</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="878787"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64815428"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="d9d9d9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -671,6 +1410,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -782,6 +1522,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -878,6 +1619,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -974,6 +1716,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1104,6 +1847,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="ctr"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1124,6 +1868,7 @@
                   </a:pPr>
                 </a:p>
               </c:txPr>
+              <c:dLblPos val="ctr"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -1142,6 +1887,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1205,11 +1951,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="38096366"/>
-        <c:axId val="85174888"/>
+        <c:axId val="18281818"/>
+        <c:axId val="78518055"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38096366"/>
+        <c:axId val="18281818"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1249,7 +1995,7 @@
             </a:ln>
           </c:spPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1275,7 +2021,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85174888"/>
+        <c:crossAx val="78518055"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1283,7 +2029,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85174888"/>
+        <c:axId val="78518055"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +2066,7 @@
                     </a:solidFill>
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>Total</a:t>
+                  <a:t>Number of Successfully passed candodates per test</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1359,741 +2105,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38096366"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="1" lang="en-GB" sz="1800" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="1" lang="en-GB" sz="1800" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>User Performance - Age 18-30</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$38</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Min</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="minus"/>
-            <c:errValType val="percentage"/>
-            <c:noEndCap val="0"/>
-            <c:val val="50"/>
-            <c:spPr>
-              <a:ln w="9360">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-          </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Browse Products</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Add Item to Basket</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>View Recommended Products</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Visit Dietary Features</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Set Preferences from Settings</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$38:$F$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$39</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Q1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c0504d"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Browse Products</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Add Item to Basket</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>View Recommended Products</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Visit Dietary Features</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Set Preferences from Settings</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$39:$F$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.75</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$40</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Median</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="9bbb59"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Browse Products</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Add Item to Basket</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>View Recommended Products</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Visit Dietary Features</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Set Preferences from Settings</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$40:$F$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$41</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Q3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="8064a2"/>
-            </a:solidFill>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="plus"/>
-            <c:errValType val="percentage"/>
-            <c:noEndCap val="0"/>
-            <c:val val="100"/>
-            <c:spPr>
-              <a:ln w="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Browse Products</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Add Item to Basket</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>View Recommended Products</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Visit Dietary Features</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Set Preferences from Settings</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$41:$F$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.75</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Max</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Browse Products</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Add Item to Basket</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>View Recommended Products</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Visit Dietary Features</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Set Preferences from Settings</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$42:$F$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="89424658"/>
-        <c:axId val="28008074"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="89424658"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="1" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Test Type</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="28008074"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="28008074"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="878787"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="1" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="1" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Total</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="9360">
-            <a:solidFill>
-              <a:srgbClr val="878787"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="89424658"/>
+        <c:crossAx val="18281818"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2132,9 +2144,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>56880</xdr:colOff>
+      <xdr:colOff>56520</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:rowOff>66240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2142,8 +2154,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13163040" y="6410520"/>
-        <a:ext cx="8042040" cy="3428640"/>
+        <a:off x="13163760" y="6410520"/>
+        <a:ext cx="8041320" cy="3428280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2162,9 +2174,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>18720</xdr:colOff>
+      <xdr:colOff>18360</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>637920</xdr:rowOff>
+      <xdr:rowOff>637560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2172,8 +2184,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="13096440" y="2657520"/>
-        <a:ext cx="8070480" cy="3409560"/>
+        <a:off x="13097160" y="2657520"/>
+        <a:ext cx="8069760" cy="3409200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2292,9 +2304,9 @@
       <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.43"/>
@@ -2932,8 +2944,8 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3750,7 +3762,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>